<commit_message>
Dnevnik uređen i prekopiran u Wiki
</commit_message>
<xml_diff>
--- a/dnevnikPromjenaDokumentacije.xlsx
+++ b/dnevnikPromjenaDokumentacije.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Autori</t>
   </si>
@@ -142,6 +142,9 @@
   <si>
     <t>-arhitektura sustava (MVC)
 -dorađen ER model baze podataka</t>
+  </si>
+  <si>
+    <t>0.6</t>
   </si>
 </sst>
 </file>
@@ -356,6 +359,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -365,33 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -400,9 +406,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:E49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,12 +739,12 @@
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
@@ -750,582 +753,582 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="21"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="22"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="22"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="9"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="9"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="9"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="11" t="s">
+      <c r="A26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="9"/>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="9"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="9"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="9"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="10"/>
+      <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="9"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="9"/>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="9"/>
+      <c r="G35" s="19"/>
     </row>
     <row r="36" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="14"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="9"/>
+      <c r="G36" s="19"/>
     </row>
     <row r="37" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="6"/>
-      <c r="G37" s="10"/>
+      <c r="G37" s="20"/>
     </row>
     <row r="38" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
       <c r="F38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="9"/>
+      <c r="G39" s="19"/>
     </row>
     <row r="40" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="14"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="9"/>
+      <c r="G40" s="19"/>
     </row>
     <row r="41" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="9"/>
+      <c r="G41" s="19"/>
     </row>
     <row r="42" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="16"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="14"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="9"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="19"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="6"/>
-      <c r="G43" s="10"/>
+      <c r="G43" s="20"/>
     </row>
     <row r="44" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11"/>
       <c r="F44" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="16"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="9"/>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="16"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="14"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="9"/>
+      <c r="G46" s="19"/>
     </row>
     <row r="47" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="16"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="5"/>
-      <c r="G47" s="9"/>
+      <c r="G47" s="19"/>
     </row>
     <row r="48" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="16"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="9"/>
+      <c r="G48" s="19"/>
     </row>
     <row r="49" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="10"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="19"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="10"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="13"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G51" s="9"/>
+      <c r="G51" s="19"/>
     </row>
     <row r="52" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="16"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="9"/>
+      <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="16"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="9"/>
+      <c r="G53" s="19"/>
     </row>
     <row r="54" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="16"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="14"/>
       <c r="F54" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G54" s="9"/>
+      <c r="G54" s="19"/>
     </row>
     <row r="55" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="19"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G55" s="10"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1342,25 +1345,6 @@
     <row r="68" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:E19"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B20:E25"/>
-    <mergeCell ref="G20:G25"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:E13"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:E31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:E37"/>
-    <mergeCell ref="G32:G37"/>
     <mergeCell ref="A38:A43"/>
     <mergeCell ref="B38:E43"/>
     <mergeCell ref="G38:G43"/>
@@ -1370,6 +1354,25 @@
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="B44:E49"/>
     <mergeCell ref="G44:G49"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:E31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:E37"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B20:E25"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:E13"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:E19"/>
+    <mergeCell ref="G14:G19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F55">

</xml_diff>

<commit_message>
Jobs route -> gotovo Search reservation -> gotovo
</commit_message>
<xml_diff>
--- a/dnevnikPromjenaDokumentacije.xlsx
+++ b/dnevnikPromjenaDokumentacije.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Autori</t>
   </si>
@@ -221,13 +221,22 @@
     <t>-isješak programskog koda vezan za temeljnu funkcionalnost sustava</t>
   </si>
   <si>
-    <t>16.1.2018.</t>
-  </si>
-  <si>
     <t>14.1.201</t>
   </si>
   <si>
     <t>13.1.2018.</t>
+  </si>
+  <si>
+    <t>Paulinović, Galić</t>
+  </si>
+  <si>
+    <t>Kravrščan, Paulinović</t>
+  </si>
+  <si>
+    <t>Krmpotić-Đurđević, Modrušan, Galić</t>
+  </si>
+  <si>
+    <t>Sodić, Krmpotić-Đurđević</t>
   </si>
 </sst>
 </file>
@@ -421,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -487,6 +496,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,8 +508,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,12 +849,12 @@
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
@@ -854,10 +872,10 @@
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
@@ -867,8 +885,8 @@
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="19"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="24"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
@@ -876,8 +894,8 @@
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
@@ -885,8 +903,8 @@
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
@@ -894,8 +912,8 @@
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="19"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
@@ -903,8 +921,8 @@
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="25"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
@@ -916,10 +934,10 @@
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="24" t="s">
         <v>13</v>
       </c>
     </row>
@@ -929,8 +947,8 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="24"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
@@ -938,8 +956,8 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="24"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
@@ -947,8 +965,8 @@
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="19"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
@@ -956,8 +974,8 @@
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="24"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
@@ -965,8 +983,8 @@
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="25"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
@@ -978,8 +996,8 @@
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="4" t="s">
-        <v>2</v>
+      <c r="F14" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>14</v>
@@ -991,9 +1009,7 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1002,7 +1018,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1011,7 +1027,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="19"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1020,7 +1036,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1029,7 +1045,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1042,7 +1058,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="11" t="s">
@@ -1055,7 +1071,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1064,7 +1080,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1073,7 +1089,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1082,7 +1098,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="19"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1091,7 +1107,7 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="6"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1104,8 +1120,8 @@
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="4" t="s">
-        <v>5</v>
+      <c r="F26" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>23</v>
@@ -1117,9 +1133,7 @@
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="F27" s="12"/>
       <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1128,7 +1142,7 @@
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="12"/>
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1137,7 +1151,7 @@
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1146,7 +1160,7 @@
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="19"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1155,7 +1169,7 @@
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="6"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1168,8 +1182,8 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="4" t="s">
-        <v>3</v>
+      <c r="F32" s="27" t="s">
+        <v>65</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>33</v>
@@ -1181,9 +1195,7 @@
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="19"/>
-      <c r="F33" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="F33" s="28"/>
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1192,9 +1204,7 @@
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="F34" s="28"/>
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1203,7 +1213,7 @@
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="19"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1212,7 +1222,7 @@
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="12"/>
     </row>
     <row r="37" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1221,7 +1231,7 @@
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="29"/>
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1234,8 +1244,8 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="16"/>
-      <c r="F38" s="4" t="s">
-        <v>2</v>
+      <c r="F38" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>32</v>
@@ -1247,7 +1257,7 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="19"/>
-      <c r="F39" s="5"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1256,7 +1266,7 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="19"/>
-      <c r="F40" s="5"/>
+      <c r="F40" s="12"/>
       <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1265,7 +1275,7 @@
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="19"/>
-      <c r="F41" s="5"/>
+      <c r="F41" s="12"/>
       <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1274,7 +1284,7 @@
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="5"/>
+      <c r="F42" s="12"/>
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1283,7 +1293,7 @@
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="6"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="13"/>
     </row>
     <row r="44" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1296,8 +1306,8 @@
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
-      <c r="F44" s="4" t="s">
-        <v>1</v>
+      <c r="F44" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="G44" s="11" t="s">
         <v>29</v>
@@ -1309,9 +1319,7 @@
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="19"/>
-      <c r="F45" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="F45" s="12"/>
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1320,7 +1328,7 @@
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="19"/>
-      <c r="F46" s="5"/>
+      <c r="F46" s="12"/>
       <c r="G46" s="12"/>
     </row>
     <row r="47" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1329,7 +1337,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="19"/>
-      <c r="F47" s="5"/>
+      <c r="F47" s="12"/>
       <c r="G47" s="12"/>
     </row>
     <row r="48" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1338,7 +1346,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="19"/>
-      <c r="F48" s="5"/>
+      <c r="F48" s="12"/>
       <c r="G48" s="12"/>
     </row>
     <row r="49" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1347,7 +1355,7 @@
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
       <c r="E49" s="22"/>
-      <c r="F49" s="6"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="13"/>
     </row>
     <row r="50" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1752,7 +1760,7 @@
         <v>5</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1814,7 +1822,7 @@
         <v>4</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1876,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2108,7 +2116,61 @@
     <row r="217" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="218" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="63">
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:E43"/>
+    <mergeCell ref="G38:G43"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="B50:E55"/>
+    <mergeCell ref="G50:G55"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:E49"/>
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="F38:F43"/>
+    <mergeCell ref="F44:F49"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:E31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:E37"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="F32:F37"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B20:E25"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:E13"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="F20:F25"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:E19"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="A56:A61"/>
+    <mergeCell ref="B56:E61"/>
+    <mergeCell ref="G56:G61"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:E67"/>
+    <mergeCell ref="G62:G67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="B68:E73"/>
+    <mergeCell ref="G68:G73"/>
+    <mergeCell ref="A74:A79"/>
+    <mergeCell ref="B74:E79"/>
+    <mergeCell ref="G74:G79"/>
+    <mergeCell ref="A80:A85"/>
+    <mergeCell ref="B80:E85"/>
+    <mergeCell ref="G80:G85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="B86:E91"/>
+    <mergeCell ref="G86:G91"/>
     <mergeCell ref="A104:A109"/>
     <mergeCell ref="B104:E109"/>
     <mergeCell ref="G104:G109"/>
@@ -2118,55 +2180,9 @@
     <mergeCell ref="A98:A103"/>
     <mergeCell ref="B98:E103"/>
     <mergeCell ref="G98:G103"/>
-    <mergeCell ref="A80:A85"/>
-    <mergeCell ref="B80:E85"/>
-    <mergeCell ref="G80:G85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="B86:E91"/>
-    <mergeCell ref="G86:G91"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="B68:E73"/>
-    <mergeCell ref="G68:G73"/>
-    <mergeCell ref="A74:A79"/>
-    <mergeCell ref="B74:E79"/>
-    <mergeCell ref="G74:G79"/>
-    <mergeCell ref="A56:A61"/>
-    <mergeCell ref="B56:E61"/>
-    <mergeCell ref="G56:G61"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:E67"/>
-    <mergeCell ref="G62:G67"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:E19"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B20:E25"/>
-    <mergeCell ref="G20:G25"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:E13"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:E31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:E37"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B38:E43"/>
-    <mergeCell ref="G38:G43"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="B50:E55"/>
-    <mergeCell ref="G50:G55"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:E49"/>
-    <mergeCell ref="G44:G49"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F50:F109">
       <formula1>Autori</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>